<commit_message>
Modified Old TypeChecker - deleted ImpAssign tests and fixed a few others.
</commit_message>
<xml_diff>
--- a/Quorum3/Library/Tests/TypeChecker/Type System.xlsx
+++ b/Quorum3/Library/Tests/TypeChecker/Type System.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
-  <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr codeName="ThisWorkbook" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="640" yWindow="600" windowWidth="29580" windowHeight="18420"/>
+    <workbookView xWindow="645" yWindow="600" windowWidth="29580" windowHeight="16440"/>
   </bookViews>
   <sheets>
     <sheet name="Quorum 3.0" sheetId="1" r:id="rId1"/>
     <sheet name="VBA Code for Hyperlinks" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -1857,6 +1857,7 @@
       <sz val="10"/>
       <color theme="11"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -2404,67 +2405,67 @@
   <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:AW114"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F62" sqref="F62"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="200" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.95" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="10.1640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="4.5" style="2" customWidth="1"/>
-    <col min="4" max="5" width="34.6640625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="3.6640625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="10.1640625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="4.5" style="3" customWidth="1"/>
-    <col min="10" max="11" width="34.6640625" style="3" customWidth="1"/>
-    <col min="12" max="12" width="3.6640625" style="3" customWidth="1"/>
-    <col min="13" max="13" width="12.6640625" style="3" customWidth="1"/>
-    <col min="14" max="14" width="10.1640625" style="3" customWidth="1"/>
-    <col min="15" max="15" width="4.5" style="3" customWidth="1"/>
-    <col min="16" max="17" width="34.6640625" style="3" customWidth="1"/>
-    <col min="18" max="18" width="3.6640625" style="3" customWidth="1"/>
-    <col min="19" max="19" width="12.6640625" style="3" customWidth="1"/>
-    <col min="20" max="20" width="10.1640625" style="3" customWidth="1"/>
-    <col min="21" max="21" width="4.5" style="3" customWidth="1"/>
-    <col min="22" max="23" width="34.6640625" style="3" customWidth="1"/>
-    <col min="24" max="24" width="3.6640625" style="3" customWidth="1"/>
-    <col min="25" max="25" width="12.6640625" style="3" customWidth="1"/>
-    <col min="26" max="26" width="10.1640625" style="3" customWidth="1"/>
-    <col min="27" max="27" width="4.5" style="3" customWidth="1"/>
-    <col min="28" max="29" width="34.6640625" style="3" customWidth="1"/>
-    <col min="30" max="30" width="3.6640625" style="3" customWidth="1"/>
-    <col min="31" max="31" width="12.6640625" style="3" customWidth="1"/>
-    <col min="32" max="32" width="10.1640625" style="3" customWidth="1"/>
-    <col min="33" max="33" width="4.5" style="3" customWidth="1"/>
-    <col min="34" max="35" width="34.6640625" style="3" customWidth="1"/>
-    <col min="36" max="36" width="3.6640625" style="3" customWidth="1"/>
-    <col min="37" max="37" width="12.6640625" style="3" customWidth="1"/>
-    <col min="38" max="38" width="10.1640625" style="3" customWidth="1"/>
-    <col min="39" max="39" width="4.5" style="3" customWidth="1"/>
-    <col min="40" max="41" width="34.6640625" style="3" customWidth="1"/>
-    <col min="42" max="16384" width="14.5" style="3"/>
+    <col min="1" max="1" width="12.7109375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="4.42578125" style="2" customWidth="1"/>
+    <col min="4" max="5" width="34.7109375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="3.7109375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="4.42578125" style="3" customWidth="1"/>
+    <col min="10" max="11" width="34.7109375" style="3" customWidth="1"/>
+    <col min="12" max="12" width="3.7109375" style="3" customWidth="1"/>
+    <col min="13" max="13" width="12.7109375" style="3" customWidth="1"/>
+    <col min="14" max="14" width="10.140625" style="3" customWidth="1"/>
+    <col min="15" max="15" width="4.42578125" style="3" customWidth="1"/>
+    <col min="16" max="17" width="34.7109375" style="3" customWidth="1"/>
+    <col min="18" max="18" width="3.7109375" style="3" customWidth="1"/>
+    <col min="19" max="19" width="12.7109375" style="3" customWidth="1"/>
+    <col min="20" max="20" width="10.140625" style="3" customWidth="1"/>
+    <col min="21" max="21" width="4.42578125" style="3" customWidth="1"/>
+    <col min="22" max="23" width="34.7109375" style="3" customWidth="1"/>
+    <col min="24" max="24" width="3.7109375" style="3" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="3" customWidth="1"/>
+    <col min="26" max="26" width="10.140625" style="3" customWidth="1"/>
+    <col min="27" max="27" width="4.42578125" style="3" customWidth="1"/>
+    <col min="28" max="29" width="34.7109375" style="3" customWidth="1"/>
+    <col min="30" max="30" width="3.7109375" style="3" customWidth="1"/>
+    <col min="31" max="31" width="12.7109375" style="3" customWidth="1"/>
+    <col min="32" max="32" width="10.140625" style="3" customWidth="1"/>
+    <col min="33" max="33" width="4.42578125" style="3" customWidth="1"/>
+    <col min="34" max="35" width="34.7109375" style="3" customWidth="1"/>
+    <col min="36" max="36" width="3.7109375" style="3" customWidth="1"/>
+    <col min="37" max="37" width="12.7109375" style="3" customWidth="1"/>
+    <col min="38" max="38" width="10.140625" style="3" customWidth="1"/>
+    <col min="39" max="39" width="4.42578125" style="3" customWidth="1"/>
+    <col min="40" max="41" width="34.7109375" style="3" customWidth="1"/>
+    <col min="42" max="16384" width="14.42578125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:49" ht="17">
+    <row r="1" spans="1:49" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:49" ht="17">
+    <row r="2" spans="1:49" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>444</v>
       </c>
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:49" ht="17">
+    <row r="3" spans="1:49" ht="18" x14ac:dyDescent="0.25">
       <c r="A3" s="8"/>
       <c r="B3" s="1"/>
     </row>
-    <row r="4" spans="1:49" s="13" customFormat="1">
+    <row r="4" spans="1:49" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="46" t="s">
         <v>445</v>
       </c>
@@ -2521,7 +2522,7 @@
       <c r="AV4" s="12"/>
       <c r="AW4" s="12"/>
     </row>
-    <row r="5" spans="1:49" ht="13" customHeight="1">
+    <row r="5" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="42" t="s">
         <v>2</v>
       </c>
@@ -2666,7 +2667,7 @@
       <c r="AV5" s="1"/>
       <c r="AW5" s="1"/>
     </row>
-    <row r="6" spans="1:49" s="11" customFormat="1" ht="13" customHeight="1">
+    <row r="6" spans="1:49" s="11" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="36" t="s">
         <v>91</v>
       </c>
@@ -2737,7 +2738,7 @@
       <c r="AV6" s="41"/>
       <c r="AW6" s="41"/>
     </row>
-    <row r="7" spans="1:49" ht="13" customHeight="1">
+    <row r="7" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="15"/>
       <c r="B7" s="19" t="s">
         <v>91</v>
@@ -2815,7 +2816,7 @@
       <c r="AT7" s="1"/>
       <c r="AU7" s="1"/>
     </row>
-    <row r="8" spans="1:49" ht="13" customHeight="1">
+    <row r="8" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="15"/>
       <c r="B8" s="19" t="s">
         <v>3</v>
@@ -2893,7 +2894,7 @@
       <c r="AU8" s="1"/>
       <c r="AV8" s="1"/>
     </row>
-    <row r="9" spans="1:49" ht="13" customHeight="1">
+    <row r="9" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="15"/>
       <c r="B9" s="25" t="s">
         <v>92</v>
@@ -2963,7 +2964,7 @@
       <c r="AO9" s="28"/>
       <c r="AT9" s="1"/>
     </row>
-    <row r="10" spans="1:49" ht="13" customHeight="1">
+    <row r="10" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="15"/>
       <c r="B10" s="25" t="s">
         <v>45</v>
@@ -3035,7 +3036,7 @@
       <c r="AT10" s="1"/>
       <c r="AU10" s="1"/>
     </row>
-    <row r="11" spans="1:49" ht="13" customHeight="1">
+    <row r="11" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="15"/>
       <c r="B11" s="25" t="s">
         <v>93</v>
@@ -3107,7 +3108,7 @@
       <c r="AT11" s="1"/>
       <c r="AU11" s="1"/>
     </row>
-    <row r="12" spans="1:49" ht="13" customHeight="1">
+    <row r="12" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="15"/>
       <c r="B12" s="25" t="s">
         <v>46</v>
@@ -3179,7 +3180,7 @@
       <c r="AT12" s="1"/>
       <c r="AU12" s="1"/>
     </row>
-    <row r="13" spans="1:49" ht="13" customHeight="1">
+    <row r="13" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="14"/>
       <c r="B13" s="19" t="s">
         <v>51</v>
@@ -3256,7 +3257,7 @@
       <c r="AT13" s="1"/>
       <c r="AU13" s="1"/>
     </row>
-    <row r="14" spans="1:49" ht="13" customHeight="1">
+    <row r="14" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="15"/>
       <c r="B14" s="25" t="s">
         <v>47</v>
@@ -3328,7 +3329,7 @@
       <c r="AT14" s="1"/>
       <c r="AU14" s="1"/>
     </row>
-    <row r="15" spans="1:49" ht="13" customHeight="1">
+    <row r="15" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="15"/>
       <c r="B15" s="25" t="s">
         <v>94</v>
@@ -3398,7 +3399,7 @@
       <c r="AO15" s="28"/>
       <c r="AT15" s="1"/>
     </row>
-    <row r="16" spans="1:49" ht="13" customHeight="1">
+    <row r="16" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="15"/>
       <c r="B16" s="19" t="s">
         <v>48</v>
@@ -3476,7 +3477,7 @@
       <c r="AT16" s="1"/>
       <c r="AU16" s="1"/>
     </row>
-    <row r="17" spans="1:49" s="11" customFormat="1" ht="13" customHeight="1">
+    <row r="17" spans="1:49" s="11" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="36" t="s">
         <v>3</v>
       </c>
@@ -3547,7 +3548,7 @@
       <c r="AV17" s="41"/>
       <c r="AW17" s="41"/>
     </row>
-    <row r="18" spans="1:49" ht="13" customHeight="1">
+    <row r="18" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="15"/>
       <c r="B18" s="19" t="s">
         <v>91</v>
@@ -3623,7 +3624,7 @@
       <c r="AT18" s="1"/>
       <c r="AU18" s="1"/>
     </row>
-    <row r="19" spans="1:49" s="5" customFormat="1" ht="13" customHeight="1">
+    <row r="19" spans="1:49" s="5" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="16"/>
       <c r="B19" s="19" t="s">
         <v>4</v>
@@ -3712,7 +3713,7 @@
       <c r="AV19" s="7"/>
       <c r="AW19" s="7"/>
     </row>
-    <row r="20" spans="1:49" ht="13" customHeight="1">
+    <row r="20" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="15"/>
       <c r="B20" s="25" t="s">
         <v>92</v>
@@ -3782,7 +3783,7 @@
       <c r="AO20" s="28"/>
       <c r="AT20" s="1"/>
     </row>
-    <row r="21" spans="1:49" ht="13" customHeight="1">
+    <row r="21" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="15"/>
       <c r="B21" s="25" t="s">
         <v>7</v>
@@ -3854,7 +3855,7 @@
       <c r="AT21" s="1"/>
       <c r="AU21" s="1"/>
     </row>
-    <row r="22" spans="1:49" ht="13" customHeight="1">
+    <row r="22" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="15"/>
       <c r="B22" s="25" t="s">
         <v>93</v>
@@ -3924,7 +3925,7 @@
       <c r="AO22" s="28"/>
       <c r="AT22" s="1"/>
     </row>
-    <row r="23" spans="1:49" ht="13" customHeight="1">
+    <row r="23" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="15"/>
       <c r="B23" s="25" t="s">
         <v>8</v>
@@ -3996,7 +3997,7 @@
       <c r="AT23" s="1"/>
       <c r="AU23" s="1"/>
     </row>
-    <row r="24" spans="1:49" ht="13" customHeight="1">
+    <row r="24" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="15"/>
       <c r="B24" s="19" t="s">
         <v>13</v>
@@ -4073,7 +4074,7 @@
       <c r="AT24" s="1"/>
       <c r="AU24" s="1"/>
     </row>
-    <row r="25" spans="1:49" ht="13" customHeight="1">
+    <row r="25" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="15"/>
       <c r="B25" s="19" t="s">
         <v>9</v>
@@ -4147,7 +4148,7 @@
       <c r="AT25" s="1"/>
       <c r="AU25" s="1"/>
     </row>
-    <row r="26" spans="1:49" ht="13" customHeight="1">
+    <row r="26" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="15"/>
       <c r="B26" s="25" t="s">
         <v>94</v>
@@ -4217,7 +4218,7 @@
       <c r="AO26" s="28"/>
       <c r="AT26" s="1"/>
     </row>
-    <row r="27" spans="1:49" ht="13" customHeight="1">
+    <row r="27" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="15"/>
       <c r="B27" s="25" t="s">
         <v>11</v>
@@ -4289,7 +4290,7 @@
       <c r="AT27" s="1"/>
       <c r="AU27" s="1"/>
     </row>
-    <row r="28" spans="1:49" s="11" customFormat="1" ht="13" customHeight="1">
+    <row r="28" spans="1:49" s="11" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="36" t="s">
         <v>92</v>
       </c>
@@ -4360,7 +4361,7 @@
       <c r="AV28" s="41"/>
       <c r="AW28" s="41"/>
     </row>
-    <row r="29" spans="1:49" ht="13" customHeight="1">
+    <row r="29" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="15"/>
       <c r="B29" s="25" t="s">
         <v>91</v>
@@ -4430,7 +4431,7 @@
       <c r="AO29" s="28"/>
       <c r="AT29" s="1"/>
     </row>
-    <row r="30" spans="1:49" ht="13" customHeight="1">
+    <row r="30" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="15"/>
       <c r="B30" s="25" t="s">
         <v>3</v>
@@ -4504,7 +4505,7 @@
       <c r="AU30" s="1"/>
       <c r="AV30" s="1"/>
     </row>
-    <row r="31" spans="1:49" ht="13" customHeight="1">
+    <row r="31" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="15"/>
       <c r="B31" s="19" t="s">
         <v>92</v>
@@ -4582,7 +4583,7 @@
       <c r="AT31" s="1"/>
       <c r="AU31" s="1"/>
     </row>
-    <row r="32" spans="1:49" ht="13" customHeight="1">
+    <row r="32" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="15"/>
       <c r="B32" s="19" t="s">
         <v>53</v>
@@ -4658,7 +4659,7 @@
       <c r="AT32" s="1"/>
       <c r="AU32" s="1"/>
     </row>
-    <row r="33" spans="1:49" ht="13" customHeight="1">
+    <row r="33" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="15"/>
       <c r="B33" s="25" t="s">
         <v>93</v>
@@ -4730,7 +4731,7 @@
       <c r="AT33" s="1"/>
       <c r="AU33" s="1"/>
     </row>
-    <row r="34" spans="1:49" ht="13" customHeight="1">
+    <row r="34" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="15"/>
       <c r="B34" s="25" t="s">
         <v>55</v>
@@ -4802,7 +4803,7 @@
       <c r="AT34" s="1"/>
       <c r="AU34" s="1"/>
     </row>
-    <row r="35" spans="1:49" ht="13" customHeight="1">
+    <row r="35" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="14"/>
       <c r="B35" s="19" t="s">
         <v>60</v>
@@ -4879,7 +4880,7 @@
       <c r="AT35" s="1"/>
       <c r="AU35" s="1"/>
     </row>
-    <row r="36" spans="1:49" ht="13" customHeight="1">
+    <row r="36" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="15"/>
       <c r="B36" s="25" t="s">
         <v>56</v>
@@ -4951,7 +4952,7 @@
       <c r="AT36" s="1"/>
       <c r="AU36" s="1"/>
     </row>
-    <row r="37" spans="1:49" ht="13" customHeight="1">
+    <row r="37" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="15"/>
       <c r="B37" s="25" t="s">
         <v>94</v>
@@ -5021,7 +5022,7 @@
       <c r="AO37" s="28"/>
       <c r="AT37" s="1"/>
     </row>
-    <row r="38" spans="1:49" ht="13" customHeight="1">
+    <row r="38" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="15"/>
       <c r="B38" s="19" t="s">
         <v>57</v>
@@ -5099,7 +5100,7 @@
       <c r="AT38" s="1"/>
       <c r="AU38" s="1"/>
     </row>
-    <row r="39" spans="1:49" s="11" customFormat="1" ht="13" customHeight="1">
+    <row r="39" spans="1:49" s="11" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="36" t="s">
         <v>7</v>
       </c>
@@ -5170,7 +5171,7 @@
       <c r="AV39" s="41"/>
       <c r="AW39" s="41"/>
     </row>
-    <row r="40" spans="1:49" customFormat="1" ht="13" customHeight="1">
+    <row r="40" spans="1:49" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="17"/>
       <c r="B40" s="30" t="s">
         <v>91</v>
@@ -5245,7 +5246,7 @@
       <c r="AN40" s="27"/>
       <c r="AO40" s="28"/>
     </row>
-    <row r="41" spans="1:49" customFormat="1" ht="13" customHeight="1">
+    <row r="41" spans="1:49" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="17"/>
       <c r="B41" s="30" t="s">
         <v>3</v>
@@ -5320,7 +5321,7 @@
       <c r="AN41" s="27"/>
       <c r="AO41" s="28"/>
     </row>
-    <row r="42" spans="1:49" customFormat="1" ht="13" customHeight="1">
+    <row r="42" spans="1:49" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="17"/>
       <c r="B42" s="19" t="s">
         <v>92</v>
@@ -5399,7 +5400,7 @@
       <c r="AN42" s="23"/>
       <c r="AO42" s="24"/>
     </row>
-    <row r="43" spans="1:49" customFormat="1" ht="13" customHeight="1">
+    <row r="43" spans="1:49" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="17"/>
       <c r="B43" s="19" t="s">
         <v>7</v>
@@ -5488,7 +5489,7 @@
       <c r="AN43" s="23"/>
       <c r="AO43" s="24"/>
     </row>
-    <row r="44" spans="1:49" customFormat="1" ht="13" customHeight="1">
+    <row r="44" spans="1:49" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="17"/>
       <c r="B44" s="25" t="s">
         <v>93</v>
@@ -5563,7 +5564,7 @@
       <c r="AN44" s="27"/>
       <c r="AO44" s="28"/>
     </row>
-    <row r="45" spans="1:49" customFormat="1" ht="13" customHeight="1">
+    <row r="45" spans="1:49" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="17"/>
       <c r="B45" s="19" t="s">
         <v>8</v>
@@ -5648,7 +5649,7 @@
       <c r="AN45" s="27"/>
       <c r="AO45" s="28"/>
     </row>
-    <row r="46" spans="1:49" customFormat="1" ht="13" customHeight="1">
+    <row r="46" spans="1:49" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="17"/>
       <c r="B46" s="19" t="s">
         <v>13</v>
@@ -5725,7 +5726,7 @@
       <c r="AN46" s="27"/>
       <c r="AO46" s="28"/>
     </row>
-    <row r="47" spans="1:49" customFormat="1" ht="13" customHeight="1">
+    <row r="47" spans="1:49" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="17"/>
       <c r="B47" s="19" t="s">
         <v>9</v>
@@ -5802,7 +5803,7 @@
       <c r="AN47" s="27"/>
       <c r="AO47" s="28"/>
     </row>
-    <row r="48" spans="1:49" customFormat="1" ht="13" customHeight="1">
+    <row r="48" spans="1:49" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="17"/>
       <c r="B48" s="30" t="s">
         <v>94</v>
@@ -5877,7 +5878,7 @@
       <c r="AN48" s="27"/>
       <c r="AO48" s="28"/>
     </row>
-    <row r="49" spans="1:49" customFormat="1" ht="13" customHeight="1">
+    <row r="49" spans="1:49" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="17"/>
       <c r="B49" s="30" t="s">
         <v>11</v>
@@ -5952,7 +5953,7 @@
       <c r="AN49" s="27"/>
       <c r="AO49" s="28"/>
     </row>
-    <row r="50" spans="1:49" s="11" customFormat="1" ht="13" customHeight="1">
+    <row r="50" spans="1:49" s="11" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="36" t="s">
         <v>93</v>
       </c>
@@ -6023,7 +6024,7 @@
       <c r="AV50" s="41"/>
       <c r="AW50" s="41"/>
     </row>
-    <row r="51" spans="1:49" ht="13" customHeight="1">
+    <row r="51" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="15"/>
       <c r="B51" s="25" t="s">
         <v>91</v>
@@ -6093,7 +6094,7 @@
       <c r="AO51" s="28"/>
       <c r="AT51" s="1"/>
     </row>
-    <row r="52" spans="1:49" ht="13" customHeight="1">
+    <row r="52" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="15"/>
       <c r="B52" s="25" t="s">
         <v>3</v>
@@ -6167,7 +6168,7 @@
       <c r="AU52" s="1"/>
       <c r="AV52" s="1"/>
     </row>
-    <row r="53" spans="1:49" ht="13" customHeight="1">
+    <row r="53" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="15"/>
       <c r="B53" s="25" t="s">
         <v>92</v>
@@ -6239,7 +6240,7 @@
       <c r="AO53" s="24"/>
       <c r="AT53" s="1"/>
     </row>
-    <row r="54" spans="1:49" ht="13" customHeight="1">
+    <row r="54" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="15"/>
       <c r="B54" s="25" t="s">
         <v>62</v>
@@ -6313,7 +6314,7 @@
       <c r="AT54" s="1"/>
       <c r="AU54" s="1"/>
     </row>
-    <row r="55" spans="1:49" ht="13" customHeight="1">
+    <row r="55" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="15"/>
       <c r="B55" s="19" t="s">
         <v>93</v>
@@ -6391,7 +6392,7 @@
       <c r="AT55" s="1"/>
       <c r="AU55" s="1"/>
     </row>
-    <row r="56" spans="1:49" ht="13" customHeight="1">
+    <row r="56" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="15"/>
       <c r="B56" s="19" t="s">
         <v>63</v>
@@ -6467,7 +6468,7 @@
       <c r="AT56" s="1"/>
       <c r="AU56" s="1"/>
     </row>
-    <row r="57" spans="1:49" ht="13" customHeight="1">
+    <row r="57" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="14"/>
       <c r="B57" s="19" t="s">
         <v>69</v>
@@ -6544,7 +6545,7 @@
       <c r="AT57" s="1"/>
       <c r="AU57" s="1"/>
     </row>
-    <row r="58" spans="1:49" ht="13" customHeight="1">
+    <row r="58" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="15"/>
       <c r="B58" s="25" t="s">
         <v>65</v>
@@ -6616,7 +6617,7 @@
       <c r="AT58" s="1"/>
       <c r="AU58" s="1"/>
     </row>
-    <row r="59" spans="1:49" ht="13" customHeight="1">
+    <row r="59" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="15"/>
       <c r="B59" s="25" t="s">
         <v>94</v>
@@ -6686,7 +6687,7 @@
       <c r="AO59" s="28"/>
       <c r="AT59" s="1"/>
     </row>
-    <row r="60" spans="1:49" ht="13" customHeight="1">
+    <row r="60" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="15"/>
       <c r="B60" s="19" t="s">
         <v>66</v>
@@ -6764,7 +6765,7 @@
       <c r="AT60" s="1"/>
       <c r="AU60" s="1"/>
     </row>
-    <row r="61" spans="1:49" s="11" customFormat="1" ht="13" customHeight="1">
+    <row r="61" spans="1:49" s="11" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="36" t="s">
         <v>8</v>
       </c>
@@ -6835,7 +6836,7 @@
       <c r="AV61" s="41"/>
       <c r="AW61" s="41"/>
     </row>
-    <row r="62" spans="1:49" ht="13" customHeight="1">
+    <row r="62" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="15"/>
       <c r="B62" s="25" t="s">
         <v>91</v>
@@ -6905,7 +6906,7 @@
       <c r="AO62" s="28"/>
       <c r="AT62" s="1"/>
     </row>
-    <row r="63" spans="1:49" ht="13" customHeight="1">
+    <row r="63" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="15"/>
       <c r="B63" s="25" t="s">
         <v>3</v>
@@ -6979,7 +6980,7 @@
       <c r="AU63" s="1"/>
       <c r="AV63" s="1"/>
     </row>
-    <row r="64" spans="1:49" ht="13" customHeight="1">
+    <row r="64" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="15"/>
       <c r="B64" s="25" t="s">
         <v>92</v>
@@ -7051,7 +7052,7 @@
       <c r="AO64" s="24"/>
       <c r="AT64" s="1"/>
     </row>
-    <row r="65" spans="1:49" ht="13" customHeight="1">
+    <row r="65" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="15"/>
       <c r="B65" s="19" t="s">
         <v>15</v>
@@ -7147,7 +7148,7 @@
       <c r="AU65" s="1"/>
       <c r="AV65" s="1"/>
     </row>
-    <row r="66" spans="1:49" ht="13" customHeight="1">
+    <row r="66" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="15"/>
       <c r="B66" s="19" t="s">
         <v>93</v>
@@ -7223,7 +7224,7 @@
       <c r="AT66" s="1"/>
       <c r="AU66" s="1"/>
     </row>
-    <row r="67" spans="1:49" ht="13" customHeight="1">
+    <row r="67" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="15"/>
       <c r="B67" s="19" t="s">
         <v>19</v>
@@ -7319,7 +7320,7 @@
       <c r="AU67" s="1"/>
       <c r="AV67" s="1"/>
     </row>
-    <row r="68" spans="1:49" ht="13" customHeight="1">
+    <row r="68" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="14"/>
       <c r="B68" s="19" t="s">
         <v>28</v>
@@ -7396,7 +7397,7 @@
       <c r="AT68" s="1"/>
       <c r="AU68" s="1"/>
     </row>
-    <row r="69" spans="1:49" ht="13" customHeight="1">
+    <row r="69" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="15"/>
       <c r="B69" s="19" t="s">
         <v>24</v>
@@ -7470,7 +7471,7 @@
       <c r="AT69" s="1"/>
       <c r="AU69" s="1"/>
     </row>
-    <row r="70" spans="1:49" ht="13" customHeight="1">
+    <row r="70" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="15"/>
       <c r="B70" s="25" t="s">
         <v>94</v>
@@ -7540,7 +7541,7 @@
       <c r="AO70" s="28"/>
       <c r="AT70" s="1"/>
     </row>
-    <row r="71" spans="1:49" ht="13" customHeight="1">
+    <row r="71" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="15"/>
       <c r="B71" s="25" t="s">
         <v>26</v>
@@ -7612,7 +7613,7 @@
       <c r="AT71" s="1"/>
       <c r="AU71" s="1"/>
     </row>
-    <row r="72" spans="1:49" s="11" customFormat="1" ht="13" customHeight="1">
+    <row r="72" spans="1:49" s="11" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="36" t="s">
         <v>13</v>
       </c>
@@ -7683,7 +7684,7 @@
       <c r="AV72" s="41"/>
       <c r="AW72" s="41"/>
     </row>
-    <row r="73" spans="1:49" ht="13" customHeight="1">
+    <row r="73" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="15"/>
       <c r="B73" s="19" t="s">
         <v>91</v>
@@ -7759,7 +7760,7 @@
       <c r="AO73" s="24"/>
       <c r="AT73" s="1"/>
     </row>
-    <row r="74" spans="1:49" ht="13" customHeight="1">
+    <row r="74" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="15"/>
       <c r="B74" s="19" t="s">
         <v>3</v>
@@ -7837,7 +7838,7 @@
       <c r="AU74" s="1"/>
       <c r="AV74" s="1"/>
     </row>
-    <row r="75" spans="1:49" ht="13" customHeight="1">
+    <row r="75" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="15"/>
       <c r="B75" s="19" t="s">
         <v>92</v>
@@ -7913,7 +7914,7 @@
       <c r="AO75" s="24"/>
       <c r="AT75" s="1"/>
     </row>
-    <row r="76" spans="1:49" ht="13" customHeight="1">
+    <row r="76" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="15"/>
       <c r="B76" s="19" t="s">
         <v>7</v>
@@ -7989,7 +7990,7 @@
       <c r="AT76" s="1"/>
       <c r="AU76" s="1"/>
     </row>
-    <row r="77" spans="1:49" ht="13" customHeight="1">
+    <row r="77" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="15"/>
       <c r="B77" s="19" t="s">
         <v>93</v>
@@ -8065,7 +8066,7 @@
       <c r="AO77" s="24"/>
       <c r="AT77" s="1"/>
     </row>
-    <row r="78" spans="1:49" ht="13" customHeight="1">
+    <row r="78" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="15"/>
       <c r="B78" s="19" t="s">
         <v>8</v>
@@ -8141,7 +8142,7 @@
       <c r="AT78" s="1"/>
       <c r="AU78" s="1"/>
     </row>
-    <row r="79" spans="1:49" ht="13" customHeight="1">
+    <row r="79" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="15"/>
       <c r="B79" s="19" t="s">
         <v>13</v>
@@ -8219,7 +8220,7 @@
       <c r="AT79" s="1"/>
       <c r="AU79" s="1"/>
     </row>
-    <row r="80" spans="1:49" ht="13" customHeight="1">
+    <row r="80" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="15"/>
       <c r="B80" s="19" t="s">
         <v>9</v>
@@ -8313,7 +8314,7 @@
       <c r="AU80" s="1"/>
       <c r="AV80" s="1"/>
     </row>
-    <row r="81" spans="1:49" ht="13" customHeight="1">
+    <row r="81" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="15"/>
       <c r="B81" s="19" t="s">
         <v>94</v>
@@ -8391,7 +8392,7 @@
       <c r="AT81" s="1"/>
       <c r="AU81" s="1"/>
     </row>
-    <row r="82" spans="1:49" ht="13" customHeight="1">
+    <row r="82" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="15"/>
       <c r="B82" s="19" t="s">
         <v>11</v>
@@ -8487,7 +8488,7 @@
       <c r="AU82" s="1"/>
       <c r="AV82" s="1"/>
     </row>
-    <row r="83" spans="1:49" s="11" customFormat="1" ht="13" customHeight="1">
+    <row r="83" spans="1:49" s="11" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="36" t="s">
         <v>9</v>
       </c>
@@ -8558,7 +8559,7 @@
       <c r="AV83" s="41"/>
       <c r="AW83" s="41"/>
     </row>
-    <row r="84" spans="1:49" ht="13" customHeight="1">
+    <row r="84" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="15"/>
       <c r="B84" s="25" t="s">
         <v>91</v>
@@ -8628,7 +8629,7 @@
       <c r="AO84" s="28"/>
       <c r="AT84" s="1"/>
     </row>
-    <row r="85" spans="1:49" ht="13" customHeight="1">
+    <row r="85" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="15"/>
       <c r="B85" s="19" t="s">
         <v>3</v>
@@ -8704,7 +8705,7 @@
       <c r="AU85" s="1"/>
       <c r="AV85" s="1"/>
     </row>
-    <row r="86" spans="1:49" ht="13" customHeight="1">
+    <row r="86" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="15"/>
       <c r="B86" s="25" t="s">
         <v>92</v>
@@ -8774,7 +8775,7 @@
       <c r="AO86" s="28"/>
       <c r="AT86" s="1"/>
     </row>
-    <row r="87" spans="1:49" ht="13" customHeight="1">
+    <row r="87" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="15"/>
       <c r="B87" s="19" t="s">
         <v>30</v>
@@ -8848,7 +8849,7 @@
       <c r="AT87" s="1"/>
       <c r="AU87" s="1"/>
     </row>
-    <row r="88" spans="1:49" ht="13" customHeight="1">
+    <row r="88" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="15"/>
       <c r="B88" s="25" t="s">
         <v>93</v>
@@ -8918,7 +8919,7 @@
       <c r="AO88" s="28"/>
       <c r="AT88" s="1"/>
     </row>
-    <row r="89" spans="1:49" ht="13" customHeight="1">
+    <row r="89" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="15"/>
       <c r="B89" s="19" t="s">
         <v>32</v>
@@ -8992,7 +8993,7 @@
       <c r="AT89" s="1"/>
       <c r="AU89" s="1"/>
     </row>
-    <row r="90" spans="1:49" ht="13" customHeight="1">
+    <row r="90" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="15"/>
       <c r="B90" s="19" t="s">
         <v>43</v>
@@ -9066,7 +9067,7 @@
       <c r="AT90" s="1"/>
       <c r="AU90" s="1"/>
     </row>
-    <row r="91" spans="1:49" ht="13" customHeight="1">
+    <row r="91" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="15"/>
       <c r="B91" s="19" t="s">
         <v>34</v>
@@ -9162,7 +9163,7 @@
       <c r="AU91" s="1"/>
       <c r="AV91" s="1"/>
     </row>
-    <row r="92" spans="1:49" ht="13" customHeight="1">
+    <row r="92" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="15"/>
       <c r="B92" s="19" t="s">
         <v>94</v>
@@ -9238,7 +9239,7 @@
       <c r="AT92" s="1"/>
       <c r="AU92" s="1"/>
     </row>
-    <row r="93" spans="1:49" ht="13" customHeight="1">
+    <row r="93" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="15"/>
       <c r="B93" s="19" t="s">
         <v>39</v>
@@ -9334,7 +9335,7 @@
       <c r="AU93" s="1"/>
       <c r="AV93" s="1"/>
     </row>
-    <row r="94" spans="1:49" s="11" customFormat="1" ht="13" customHeight="1">
+    <row r="94" spans="1:49" s="11" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="36" t="s">
         <v>94</v>
       </c>
@@ -9405,7 +9406,7 @@
       <c r="AV94" s="41"/>
       <c r="AW94" s="41"/>
     </row>
-    <row r="95" spans="1:49" ht="13" customHeight="1">
+    <row r="95" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="15"/>
       <c r="B95" s="25" t="s">
         <v>91</v>
@@ -9475,7 +9476,7 @@
       <c r="AO95" s="28"/>
       <c r="AT95" s="1"/>
     </row>
-    <row r="96" spans="1:49" ht="13" customHeight="1">
+    <row r="96" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="15"/>
       <c r="B96" s="25" t="s">
         <v>3</v>
@@ -9549,7 +9550,7 @@
       <c r="AU96" s="1"/>
       <c r="AV96" s="1"/>
     </row>
-    <row r="97" spans="1:49" ht="13" customHeight="1">
+    <row r="97" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="15"/>
       <c r="B97" s="25" t="s">
         <v>92</v>
@@ -9619,7 +9620,7 @@
       <c r="AO97" s="28"/>
       <c r="AT97" s="1"/>
     </row>
-    <row r="98" spans="1:49" ht="13" customHeight="1">
+    <row r="98" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="15"/>
       <c r="B98" s="25" t="s">
         <v>71</v>
@@ -9691,7 +9692,7 @@
       <c r="AT98" s="1"/>
       <c r="AU98" s="1"/>
     </row>
-    <row r="99" spans="1:49" ht="13" customHeight="1">
+    <row r="99" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="15"/>
       <c r="B99" s="25" t="s">
         <v>93</v>
@@ -9761,7 +9762,7 @@
       <c r="AO99" s="28"/>
       <c r="AT99" s="1"/>
     </row>
-    <row r="100" spans="1:49" ht="13" customHeight="1">
+    <row r="100" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="15"/>
       <c r="B100" s="25" t="s">
         <v>72</v>
@@ -9833,7 +9834,7 @@
       <c r="AT100" s="1"/>
       <c r="AU100" s="1"/>
     </row>
-    <row r="101" spans="1:49" ht="13" customHeight="1">
+    <row r="101" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="15"/>
       <c r="B101" s="19" t="s">
         <v>78</v>
@@ -9907,7 +9908,7 @@
       <c r="AT101" s="1"/>
       <c r="AU101" s="1"/>
     </row>
-    <row r="102" spans="1:49" ht="13" customHeight="1">
+    <row r="102" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="15"/>
       <c r="B102" s="19" t="s">
         <v>73</v>
@@ -9983,7 +9984,7 @@
       <c r="AT102" s="1"/>
       <c r="AU102" s="1"/>
     </row>
-    <row r="103" spans="1:49" ht="13" customHeight="1">
+    <row r="103" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="15"/>
       <c r="B103" s="19" t="s">
         <v>94</v>
@@ -10061,7 +10062,7 @@
       <c r="AT103" s="1"/>
       <c r="AU103" s="1"/>
     </row>
-    <row r="104" spans="1:49" ht="13" customHeight="1">
+    <row r="104" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="15"/>
       <c r="B104" s="19" t="s">
         <v>75</v>
@@ -10139,7 +10140,7 @@
       <c r="AT104" s="1"/>
       <c r="AU104" s="1"/>
     </row>
-    <row r="105" spans="1:49" s="11" customFormat="1" ht="13" customHeight="1">
+    <row r="105" spans="1:49" s="11" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="36" t="s">
         <v>11</v>
       </c>
@@ -10210,7 +10211,7 @@
       <c r="AV105" s="41"/>
       <c r="AW105" s="41"/>
     </row>
-    <row r="106" spans="1:49" ht="13" customHeight="1">
+    <row r="106" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="18"/>
       <c r="B106" s="32" t="s">
         <v>13</v>
@@ -10284,7 +10285,7 @@
       <c r="AU106" s="1"/>
       <c r="AV106" s="1"/>
     </row>
-    <row r="108" spans="1:49" ht="13" customHeight="1">
+    <row r="108" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="2">
         <f>COUNTA(A6:A106)</f>
         <v>10</v>
@@ -10305,7 +10306,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="109" spans="1:49" ht="13" customHeight="1">
+    <row r="109" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B109" s="3" t="s">
         <v>155</v>
       </c>
@@ -10322,7 +10323,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="110" spans="1:49" ht="13" customHeight="1">
+    <row r="110" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B110" s="10" t="s">
         <v>257</v>
       </c>
@@ -10339,17 +10340,17 @@
         <v>91</v>
       </c>
     </row>
-    <row r="112" spans="1:49" ht="13" customHeight="1">
+    <row r="112" spans="1:49" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B112" s="3">
         <v>238</v>
       </c>
     </row>
-    <row r="113" spans="2:2" ht="13" customHeight="1">
+    <row r="113" spans="2:2" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B113" s="3">
         <v>325</v>
       </c>
     </row>
-    <row r="114" spans="2:2" ht="13" customHeight="1">
+    <row r="114" spans="2:2" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B114" s="3">
         <f>B113-B112+1</f>
         <v>88</v>
@@ -10923,44 +10924,44 @@
       <selection activeCell="A9" sqref="A2:A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>443</v>
       </c>

</xml_diff>